<commit_message>
A few more levels, electron animation
</commit_message>
<xml_diff>
--- a/supaplex/tiles.xlsx
+++ b/supaplex/tiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cx16\code\supaplex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2478316A-6112-449D-B973-BF529CAD4817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE675ED1-5FCD-4270-B9A9-52905031C329}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5115" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{84989C15-12F1-4459-827F-A323921D3FDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{84989C15-12F1-4459-827F-A323921D3FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,27 +309,6 @@
     <t>BaseEat7</t>
   </si>
   <si>
-    <t>ElectronEat1</t>
-  </si>
-  <si>
-    <t>ElectronEat2</t>
-  </si>
-  <si>
-    <t>ElectronEat3</t>
-  </si>
-  <si>
-    <t>ElectronEat4</t>
-  </si>
-  <si>
-    <t>ElectronEat5</t>
-  </si>
-  <si>
-    <t>ElectronEat6</t>
-  </si>
-  <si>
-    <t>ElectronEat7</t>
-  </si>
-  <si>
     <t>DiskEat1</t>
   </si>
   <si>
@@ -730,6 +709,27 @@
   </si>
   <si>
     <t>MurphyUhOh</t>
+  </si>
+  <si>
+    <t>InfotronEat1</t>
+  </si>
+  <si>
+    <t>InfotronEat2</t>
+  </si>
+  <si>
+    <t>InfotronEat3</t>
+  </si>
+  <si>
+    <t>InfotronEat4</t>
+  </si>
+  <si>
+    <t>InfotronEat5</t>
+  </si>
+  <si>
+    <t>InfotronEat6</t>
+  </si>
+  <si>
+    <t>InfotronEat7</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923964EB-53D6-4F35-B01B-870FC0CDE014}">
   <dimension ref="A1:N200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N200"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1883,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1925,7 +1925,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1967,7 +1967,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -2012,7 +2012,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -2057,7 +2057,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -2099,7 +2099,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -2183,7 +2183,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -2351,7 +2351,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C26" t="s">
         <v>22</v>
@@ -3614,7 +3614,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -4160,17 +4160,17 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>90</v>
+        <v>224</v>
       </c>
       <c r="C69" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D69">
         <v>5</v>
       </c>
       <c r="G69">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H69">
         <f t="shared" si="8"/>
@@ -4178,23 +4178,23 @@
       </c>
       <c r="I69">
         <f t="shared" si="9"/>
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="J69">
         <f t="shared" si="10"/>
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="K69">
         <f t="shared" si="12"/>
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="L69" t="str">
         <f t="shared" si="11"/>
-        <v>:02008600858073</v>
+        <v>:02008600353013</v>
       </c>
       <c r="N69" t="str">
         <f t="shared" si="13"/>
-        <v>tileElectronEat1: +tileDef  67, ELECTR_ADDR, 5, ELECTR_PAL, 0</v>
+        <v>tileInfotronEat1: +tileDef  67, INFOTR_ADDR, 5, INFOTR_PAL, 0</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -4202,17 +4202,17 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>91</v>
+        <v>225</v>
       </c>
       <c r="C70" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D70">
         <v>6</v>
       </c>
       <c r="G70">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H70">
         <f t="shared" si="8"/>
@@ -4220,23 +4220,23 @@
       </c>
       <c r="I70">
         <f t="shared" si="9"/>
-        <v>134</v>
+        <v>54</v>
       </c>
       <c r="J70">
         <f t="shared" si="10"/>
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="K70">
         <f t="shared" si="12"/>
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="L70" t="str">
         <f t="shared" si="11"/>
-        <v>:02008800868070</v>
+        <v>:02008800363010</v>
       </c>
       <c r="N70" t="str">
         <f t="shared" si="13"/>
-        <v>tileElectronEat2: +tileDef  68, ELECTR_ADDR, 6, ELECTR_PAL, 0</v>
+        <v>tileInfotronEat2: +tileDef  68, INFOTR_ADDR, 6, INFOTR_PAL, 0</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -4244,17 +4244,17 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>92</v>
+        <v>226</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D71">
         <v>7</v>
       </c>
       <c r="G71">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H71">
         <f t="shared" si="8"/>
@@ -4262,23 +4262,23 @@
       </c>
       <c r="I71">
         <f t="shared" si="9"/>
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="J71">
         <f t="shared" si="10"/>
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="K71">
         <f t="shared" si="12"/>
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="L71" t="str">
         <f t="shared" si="11"/>
-        <v>:02008A0087806D</v>
+        <v>:02008A0037300D</v>
       </c>
       <c r="N71" t="str">
         <f t="shared" si="13"/>
-        <v>tileElectronEat3: +tileDef  69, ELECTR_ADDR, 7, ELECTR_PAL, 0</v>
+        <v>tileInfotronEat3: +tileDef  69, INFOTR_ADDR, 7, INFOTR_PAL, 0</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -4286,17 +4286,17 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>227</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D72">
         <v>8</v>
       </c>
       <c r="G72">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H72">
         <f t="shared" si="8"/>
@@ -4304,23 +4304,23 @@
       </c>
       <c r="I72">
         <f t="shared" si="9"/>
-        <v>136</v>
+        <v>56</v>
       </c>
       <c r="J72">
         <f t="shared" si="10"/>
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="K72">
         <f t="shared" si="12"/>
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="L72" t="str">
         <f t="shared" si="11"/>
-        <v>:02008C0088806A</v>
+        <v>:02008C0038300A</v>
       </c>
       <c r="N72" t="str">
         <f t="shared" si="13"/>
-        <v>tileElectronEat4: +tileDef  70, ELECTR_ADDR, 8, ELECTR_PAL, 0</v>
+        <v>tileInfotronEat4: +tileDef  70, INFOTR_ADDR, 8, INFOTR_PAL, 0</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -4328,17 +4328,17 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>228</v>
       </c>
       <c r="C73" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D73">
         <v>9</v>
       </c>
       <c r="G73">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H73">
         <f t="shared" si="8"/>
@@ -4346,23 +4346,23 @@
       </c>
       <c r="I73">
         <f t="shared" si="9"/>
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="J73">
         <f t="shared" si="10"/>
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="K73">
         <f t="shared" si="12"/>
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="L73" t="str">
         <f t="shared" si="11"/>
-        <v>:02008E00898067</v>
+        <v>:02008E00393007</v>
       </c>
       <c r="N73" t="str">
         <f t="shared" si="13"/>
-        <v>tileElectronEat5: +tileDef  71, ELECTR_ADDR, 9, ELECTR_PAL, 0</v>
+        <v>tileInfotronEat5: +tileDef  71, INFOTR_ADDR, 9, INFOTR_PAL, 0</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -4370,17 +4370,17 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>229</v>
       </c>
       <c r="C74" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D74">
         <v>10</v>
       </c>
       <c r="G74">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H74">
         <f t="shared" si="8"/>
@@ -4388,23 +4388,23 @@
       </c>
       <c r="I74">
         <f t="shared" si="9"/>
-        <v>138</v>
+        <v>58</v>
       </c>
       <c r="J74">
         <f t="shared" si="10"/>
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="K74">
         <f t="shared" si="12"/>
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="L74" t="str">
         <f t="shared" si="11"/>
-        <v>:020090008A8064</v>
+        <v>:020090003A3004</v>
       </c>
       <c r="N74" t="str">
         <f t="shared" si="13"/>
-        <v>tileElectronEat6: +tileDef  72, ELECTR_ADDR, 10, ELECTR_PAL, 0</v>
+        <v>tileInfotronEat6: +tileDef  72, INFOTR_ADDR, 10, INFOTR_PAL, 0</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -4412,17 +4412,17 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
+        <v>230</v>
       </c>
       <c r="C75" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D75">
         <v>11</v>
       </c>
       <c r="G75">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H75">
         <f t="shared" si="8"/>
@@ -4430,23 +4430,23 @@
       </c>
       <c r="I75">
         <f t="shared" si="9"/>
-        <v>139</v>
+        <v>59</v>
       </c>
       <c r="J75">
         <f t="shared" si="10"/>
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="K75">
         <f t="shared" si="12"/>
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="L75" t="str">
         <f t="shared" si="11"/>
-        <v>:020092008B8061</v>
+        <v>:020092003B3001</v>
       </c>
       <c r="N75" t="str">
         <f t="shared" si="13"/>
-        <v>tileElectronEat7: +tileDef  73, ELECTR_ADDR, 11, ELECTR_PAL, 0</v>
+        <v>tileInfotronEat7: +tileDef  73, INFOTR_ADDR, 11, INFOTR_PAL, 0</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -4454,7 +4454,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C76" t="s">
         <v>12</v>
@@ -4496,7 +4496,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C77" t="s">
         <v>12</v>
@@ -4538,7 +4538,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C78" t="s">
         <v>12</v>
@@ -4580,7 +4580,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C79" t="s">
         <v>12</v>
@@ -4622,7 +4622,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
         <v>12</v>
@@ -4664,7 +4664,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C81" t="s">
         <v>12</v>
@@ -4706,7 +4706,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C82" t="s">
         <v>12</v>
@@ -4748,7 +4748,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C83" t="s">
         <v>18</v>
@@ -4790,7 +4790,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C84" t="s">
         <v>18</v>
@@ -4832,7 +4832,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C85" t="s">
         <v>18</v>
@@ -4874,7 +4874,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C86" t="s">
         <v>18</v>
@@ -4916,7 +4916,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C87" t="s">
         <v>18</v>
@@ -4958,7 +4958,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C88" t="s">
         <v>18</v>
@@ -5000,7 +5000,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C89" t="s">
         <v>18</v>
@@ -5042,7 +5042,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C90" t="s">
         <v>18</v>
@@ -5084,7 +5084,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C91" t="s">
         <v>18</v>
@@ -5126,7 +5126,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C92" t="s">
         <v>18</v>
@@ -5168,7 +5168,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C93" t="s">
         <v>18</v>
@@ -5210,7 +5210,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C94" t="s">
         <v>18</v>
@@ -5252,7 +5252,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C95" t="s">
         <v>18</v>
@@ -5294,7 +5294,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C96" t="s">
         <v>18</v>
@@ -5336,7 +5336,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C97" t="s">
         <v>23</v>
@@ -5381,7 +5381,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C98" t="s">
         <v>23</v>
@@ -5423,7 +5423,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C99" t="s">
         <v>23</v>
@@ -5465,7 +5465,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C100" t="s">
         <v>23</v>
@@ -5507,7 +5507,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C101" t="s">
         <v>23</v>
@@ -5555,7 +5555,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C102" t="s">
         <v>23</v>
@@ -5600,7 +5600,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
@@ -5645,7 +5645,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C104" t="s">
         <v>23</v>
@@ -5690,7 +5690,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C105" t="s">
         <v>20</v>
@@ -5732,7 +5732,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C106" t="s">
         <v>20</v>
@@ -5774,7 +5774,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C107" t="s">
         <v>20</v>
@@ -5816,7 +5816,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C108" t="s">
         <v>20</v>
@@ -5858,7 +5858,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C109" t="s">
         <v>20</v>
@@ -5900,7 +5900,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C110" t="s">
         <v>20</v>
@@ -5942,7 +5942,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C111" t="s">
         <v>20</v>
@@ -5984,7 +5984,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C112" t="s">
         <v>20</v>
@@ -6026,7 +6026,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C113" t="s">
         <v>20</v>
@@ -6068,7 +6068,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C114" t="s">
         <v>20</v>
@@ -6110,7 +6110,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C115" t="s">
         <v>20</v>
@@ -6152,7 +6152,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C116" t="s">
         <v>20</v>
@@ -6194,7 +6194,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C117" t="s">
         <v>20</v>
@@ -6236,7 +6236,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C118" t="s">
         <v>20</v>
@@ -6278,7 +6278,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C119" t="s">
         <v>20</v>
@@ -6320,7 +6320,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C120" t="s">
         <v>20</v>
@@ -6362,7 +6362,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C121" t="s">
         <v>22</v>
@@ -6404,7 +6404,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C122" t="s">
         <v>22</v>
@@ -6446,7 +6446,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C123" t="s">
         <v>22</v>
@@ -6488,7 +6488,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C124" t="s">
         <v>22</v>
@@ -6530,7 +6530,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C125" t="s">
         <v>22</v>
@@ -6572,7 +6572,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C126" t="s">
         <v>22</v>
@@ -6614,7 +6614,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C127" t="s">
         <v>22</v>
@@ -6656,7 +6656,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C128" t="s">
         <v>22</v>
@@ -6698,7 +6698,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C129" t="s">
         <v>23</v>
@@ -6740,7 +6740,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C130" t="s">
         <v>23</v>
@@ -6782,7 +6782,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C131" t="s">
         <v>23</v>
@@ -6824,7 +6824,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C132" t="s">
         <v>23</v>
@@ -6866,7 +6866,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C133" t="s">
         <v>23</v>
@@ -6908,7 +6908,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C134" t="s">
         <v>23</v>
@@ -6950,7 +6950,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C135" t="s">
         <v>23</v>
@@ -6992,7 +6992,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C136" t="s">
         <v>23</v>
@@ -7034,7 +7034,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C137" t="s">
         <v>23</v>
@@ -7079,7 +7079,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C138" t="s">
         <v>23</v>
@@ -7124,7 +7124,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C139" t="s">
         <v>23</v>
@@ -7169,7 +7169,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C140" t="s">
         <v>23</v>
@@ -7214,7 +7214,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C141" t="s">
         <v>23</v>
@@ -7259,7 +7259,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C142" t="s">
         <v>23</v>
@@ -7304,7 +7304,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C143" t="s">
         <v>23</v>
@@ -7349,7 +7349,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C144" t="s">
         <v>23</v>
@@ -7394,7 +7394,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C145" t="s">
         <v>7</v>
@@ -7436,7 +7436,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C146" t="s">
         <v>7</v>
@@ -7478,7 +7478,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C147" t="s">
         <v>7</v>
@@ -7520,7 +7520,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C148" t="s">
         <v>7</v>
@@ -7562,7 +7562,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C149" t="s">
         <v>7</v>
@@ -7604,7 +7604,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C150" t="s">
         <v>7</v>
@@ -7646,7 +7646,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C151" t="s">
         <v>7</v>
@@ -7688,7 +7688,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C152" t="s">
         <v>7</v>
@@ -7730,7 +7730,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C153" t="s">
         <v>7</v>
@@ -7775,7 +7775,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C154" t="s">
         <v>7</v>
@@ -7820,7 +7820,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C155" t="s">
         <v>7</v>
@@ -7865,7 +7865,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C156" t="s">
         <v>7</v>
@@ -7910,7 +7910,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C157" t="s">
         <v>7</v>
@@ -7955,7 +7955,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C158" t="s">
         <v>7</v>
@@ -8000,7 +8000,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C159" t="s">
         <v>7</v>
@@ -8045,7 +8045,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C160" t="s">
         <v>7</v>
@@ -8090,7 +8090,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C161" t="s">
         <v>12</v>
@@ -8132,7 +8132,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C162" t="s">
         <v>12</v>
@@ -8174,7 +8174,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C163" t="s">
         <v>12</v>
@@ -8219,7 +8219,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C164" t="s">
         <v>12</v>
@@ -8261,7 +8261,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C165" t="s">
         <v>12</v>
@@ -8303,7 +8303,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C166" t="s">
         <v>12</v>
@@ -8345,7 +8345,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C167" t="s">
         <v>12</v>
@@ -8390,7 +8390,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C168" t="s">
         <v>12</v>
@@ -8432,7 +8432,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C169" t="s">
         <v>24</v>
@@ -8474,7 +8474,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C170" t="s">
         <v>24</v>
@@ -8516,7 +8516,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C171" t="s">
         <v>24</v>
@@ -8558,7 +8558,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C172" t="s">
         <v>24</v>
@@ -8600,7 +8600,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C173" t="s">
         <v>24</v>
@@ -8648,7 +8648,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C174" t="s">
         <v>24</v>
@@ -8696,7 +8696,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C175" t="s">
         <v>24</v>
@@ -8744,7 +8744,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C176" t="s">
         <v>24</v>
@@ -8792,7 +8792,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C177" t="s">
         <v>19</v>
@@ -8834,7 +8834,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C178" t="s">
         <v>19</v>
@@ -8876,7 +8876,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C179" t="s">
         <v>19</v>
@@ -8918,7 +8918,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C180" t="s">
         <v>19</v>
@@ -8960,7 +8960,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C181" t="s">
         <v>19</v>
@@ -9002,7 +9002,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C182" t="s">
         <v>19</v>
@@ -9044,7 +9044,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C183" t="s">
         <v>19</v>
@@ -9086,7 +9086,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C184" t="s">
         <v>19</v>
@@ -9128,7 +9128,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C185" t="s">
         <v>23</v>
@@ -9170,7 +9170,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C186" t="s">
         <v>23</v>
@@ -9212,7 +9212,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C187" t="s">
         <v>23</v>
@@ -9254,7 +9254,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C188" t="s">
         <v>23</v>
@@ -9296,7 +9296,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C189" t="s">
         <v>23</v>
@@ -9338,7 +9338,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C190" t="s">
         <v>23</v>
@@ -9380,7 +9380,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C191" t="s">
         <v>23</v>
@@ -9422,7 +9422,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C192" t="s">
         <v>23</v>
@@ -9464,7 +9464,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C193" t="s">
         <v>23</v>
@@ -9509,7 +9509,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C194" t="s">
         <v>23</v>
@@ -9554,7 +9554,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C195" t="s">
         <v>23</v>
@@ -9599,7 +9599,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C196" t="s">
         <v>23</v>
@@ -9644,7 +9644,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C197" t="s">
         <v>23</v>
@@ -9689,7 +9689,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C198" t="s">
         <v>23</v>
@@ -9734,7 +9734,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C199" t="s">
         <v>23</v>
@@ -9779,7 +9779,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C200" t="s">
         <v>23</v>

</xml_diff>